<commit_message>
Update Listener and Extent Report
Update Listener and Extent Report
</commit_message>
<xml_diff>
--- a/src/test/Resources/datatest/CRM.xlsx
+++ b/src/test/Resources/datatest/CRM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
   <si>
     <t>EMAIL</t>
   </si>
@@ -60,12 +60,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
     </fill>
   </fills>
   <borders count="1">
@@ -80,9 +83,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,9 +371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -393,9 +397,7 @@
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>